<commit_message>
Learning Advance Control Updated
</commit_message>
<xml_diff>
--- a/Learning Advance Control.xlsx
+++ b/Learning Advance Control.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USUARIO\GR\Software Development\Learning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ECD4454-9015-4067-A6B7-0C47907C353B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28568FF9-E4C3-4287-97B2-D1D4931025DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12360" xr2:uid="{C28AFF7E-06EE-4EAA-BF3B-F70E2F389C99}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="737" uniqueCount="584">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="739" uniqueCount="585">
   <si>
     <t>Basic Syntax</t>
   </si>
@@ -2344,6 +2344,9 @@
   </si>
   <si>
     <t>HackerRank DataStructures Exercices</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -2629,7 +2632,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
@@ -2783,6 +2786,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -2795,8 +2801,8 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3338,10 +3344,10 @@
       <c r="D18" s="23"/>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B19" s="58" t="s">
+      <c r="B19" s="59" t="s">
         <v>575</v>
       </c>
-      <c r="C19" s="58"/>
+      <c r="C19" s="59"/>
       <c r="D19" s="22">
         <v>1</v>
       </c>
@@ -3352,7 +3358,7 @@
       <c r="D20" s="23"/>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B21" s="57" t="s">
+      <c r="B21" s="58" t="s">
         <v>21</v>
       </c>
       <c r="C21" s="7" t="s">
@@ -3363,7 +3369,7 @@
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B22" s="57"/>
+      <c r="B22" s="58"/>
       <c r="C22" s="7" t="s">
         <v>15</v>
       </c>
@@ -3389,7 +3395,7 @@
       </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C25" s="61" t="s">
+      <c r="C25" s="57" t="s">
         <v>18</v>
       </c>
       <c r="D25" s="22">
@@ -3397,7 +3403,7 @@
       </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C26" s="61" t="s">
+      <c r="C26" s="57" t="s">
         <v>19</v>
       </c>
       <c r="D26" s="22">
@@ -3409,10 +3415,10 @@
       <c r="D27" s="23"/>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B28" s="58" t="s">
+      <c r="B28" s="59" t="s">
         <v>583</v>
       </c>
-      <c r="C28" s="58"/>
+      <c r="C28" s="59"/>
       <c r="D28" s="22">
         <v>0</v>
       </c>
@@ -3606,7 +3612,7 @@
   <dimension ref="B2:D45"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3631,7 +3637,7 @@
       </c>
       <c r="D3" s="22">
         <f>+AVERAGE(D5,D6,D9,D10,D16,D17,D20,D21,D24,D25,D26,D27,D30,D34,D38)</f>
-        <v>4.6666666666666669E-2</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="4" spans="2:4" s="11" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -3640,7 +3646,7 @@
       <c r="D4" s="21"/>
     </row>
     <row r="5" spans="2:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="60" t="s">
+      <c r="B5" s="61" t="s">
         <v>32</v>
       </c>
       <c r="C5" s="7" t="s">
@@ -3651,7 +3657,7 @@
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B6" s="60"/>
+      <c r="B6" s="61"/>
       <c r="C6" s="7" t="s">
         <v>34</v>
       </c>
@@ -3669,24 +3675,24 @@
       <c r="D8" s="22"/>
     </row>
     <row r="9" spans="2:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="59" t="s">
+      <c r="B9" s="60" t="s">
         <v>35</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>36</v>
       </c>
       <c r="D9" s="22">
-        <v>0.15</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B10" s="59"/>
+      <c r="B10" s="60"/>
       <c r="C10" s="7" t="s">
         <v>37</v>
       </c>
       <c r="D10" s="22">
         <f>+AVERAGE(D11)</f>
-        <v>0.15</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.3">
@@ -3694,23 +3700,23 @@
         <v>38</v>
       </c>
       <c r="D11" s="24">
-        <v>0.15</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C12" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="D12" s="24">
-        <v>0</v>
+      <c r="D12" s="62" t="s">
+        <v>584</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C13" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="D13" s="24">
-        <v>0</v>
+      <c r="D13" s="62" t="s">
+        <v>584</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Directiory renamed / Recursion started
</commit_message>
<xml_diff>
--- a/Learning Advance Control.xlsx
+++ b/Learning Advance Control.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USUARIO\GR\Software Development\Learning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57A26097-2A14-4913-8A2C-B1C1DDB90DD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28EBC7C9-381A-4881-A0AE-14EAA5CEDA6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{C28AFF7E-06EE-4EAA-BF3B-F70E2F389C99}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C28AFF7E-06EE-4EAA-BF3B-F70E2F389C99}"/>
   </bookViews>
   <sheets>
     <sheet name="Language" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="740" uniqueCount="586">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="748" uniqueCount="594">
   <si>
     <t>Basic Syntax</t>
   </si>
@@ -2351,12 +2351,36 @@
   <si>
     <t>Algoritmos de ordenamiento</t>
   </si>
+  <si>
+    <t>Prefix Sums</t>
+  </si>
+  <si>
+    <t>Sliding Window</t>
+  </si>
+  <si>
+    <t>Two pointers</t>
+  </si>
+  <si>
+    <t>Decision Trees</t>
+  </si>
+  <si>
+    <t>For Later on…</t>
+  </si>
+  <si>
+    <t>Dynamic Programming</t>
+  </si>
+  <si>
+    <t>DFS &amp; BFS (In depth)</t>
+  </si>
+  <si>
+    <t>4. More complex specific cases</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="28" x14ac:knownFonts="1">
+  <fonts count="30" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2571,8 +2595,24 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color rgb="FFCCCCFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="9" tint="0.39997558519241921"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2621,6 +2661,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -2635,7 +2681,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
@@ -2798,14 +2844,23 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2816,6 +2871,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFCCCCFF"/>
       <color rgb="FF441D61"/>
       <color rgb="FF00DE64"/>
       <color rgb="FF7EBA56"/>
@@ -3195,16 +3251,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E55BE2DC-6D03-4737-9A16-12A22A3E1488}">
-  <dimension ref="B2:H57"/>
+  <dimension ref="B2:H60"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" outlineLevelRow="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.5546875" customWidth="1"/>
-    <col min="2" max="2" width="18.77734375" style="5" customWidth="1"/>
+    <col min="1" max="1" width="11.109375" customWidth="1"/>
+    <col min="2" max="2" width="29.21875" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23.77734375" style="6" customWidth="1"/>
     <col min="4" max="4" width="10.5546875" style="5" customWidth="1"/>
     <col min="5" max="5" width="1.77734375" customWidth="1"/>
@@ -3223,8 +3279,8 @@
         <v>57</v>
       </c>
       <c r="D3" s="22">
-        <f>+AVERAGE(D5,D6,D14,D16,D17,D15,D21,D22,D23,D24,D26,D27,D31,D32,D33,D34,D35,D36,D37,D38,D39,D40,D25)</f>
-        <v>0.51586956521739136</v>
+        <f>+AVERAGE(D5,D6,D14,D16,D17,D15,D21,D22,D23,D24,D26,D27,D31,D36,D37,D38,D39)</f>
+        <v>0.63529411764705879</v>
       </c>
     </row>
     <row r="4" spans="2:8" s="11" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -3252,7 +3308,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:8" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="C7" s="13" t="s">
         <v>2</v>
       </c>
@@ -3260,7 +3316,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:8" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="C8" s="13" t="s">
         <v>3</v>
       </c>
@@ -3269,7 +3325,7 @@
       </c>
       <c r="H8" s="26"/>
     </row>
-    <row r="9" spans="2:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:8" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="C9" s="13" t="s">
         <v>4</v>
       </c>
@@ -3277,7 +3333,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:8" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="C10" s="13" t="s">
         <v>5</v>
       </c>
@@ -3285,7 +3341,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:8" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="C11" s="13" t="s">
         <v>6</v>
       </c>
@@ -3293,7 +3349,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:8" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="C12" s="13" t="s">
         <v>11</v>
       </c>
@@ -3301,7 +3357,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:8" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="C13" s="13" t="s">
         <v>7</v>
       </c>
@@ -3310,7 +3366,7 @@
       </c>
       <c r="F13" s="26"/>
     </row>
-    <row r="14" spans="2:8" collapsed="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C14" s="7" t="s">
         <v>8</v>
       </c>
@@ -3347,10 +3403,10 @@
       <c r="D18" s="23"/>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B19" s="60" t="s">
+      <c r="B19" s="65" t="s">
         <v>574</v>
       </c>
-      <c r="C19" s="60"/>
+      <c r="C19" s="65"/>
       <c r="D19" s="22">
         <v>1</v>
       </c>
@@ -3401,9 +3457,8 @@
         <v>584</v>
       </c>
       <c r="D25" s="22">
-        <v>0.6</v>
-      </c>
-      <c r="E25" s="56"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C26" s="57" t="s">
@@ -3412,6 +3467,7 @@
       <c r="D26" s="22">
         <v>0.1</v>
       </c>
+      <c r="E26" s="56"/>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C27" s="57" t="s">
@@ -3426,10 +3482,10 @@
       <c r="D28" s="23"/>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B29" s="60" t="s">
+      <c r="B29" s="65" t="s">
         <v>582</v>
       </c>
-      <c r="C29" s="60"/>
+      <c r="C29" s="65"/>
       <c r="D29" s="22">
         <v>0</v>
       </c>
@@ -3443,53 +3499,54 @@
         <v>20</v>
       </c>
       <c r="C31" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D31" s="22">
+        <f>+AVERAGE(D32:D35)</f>
+        <v>0.15000000000000002</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="C32" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="D31" s="22">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C32" s="7" t="s">
+      <c r="D32" s="22">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="C33" s="13" t="s">
         <v>23</v>
-      </c>
-      <c r="D32" s="22">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="33" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C33" s="7" t="s">
-        <v>24</v>
       </c>
       <c r="D33" s="22">
         <v>0.15</v>
       </c>
     </row>
-    <row r="34" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C34" s="7" t="s">
-        <v>25</v>
+    <row r="34" spans="2:4" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="C34" s="13" t="s">
+        <v>24</v>
       </c>
       <c r="D34" s="22">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="C35" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D35" s="22">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C36" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D36" s="22">
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C35" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D35" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C36" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D36" s="22">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="37" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C37" s="7" t="s">
         <v>28</v>
       </c>
@@ -3497,7 +3554,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="38" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C38" s="7" t="s">
         <v>580</v>
       </c>
@@ -3505,7 +3562,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="39" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C39" s="7" t="s">
         <v>581</v>
       </c>
@@ -3513,75 +3570,129 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C40" s="7" t="s">
+    <row r="40" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C40" s="7"/>
+      <c r="D40" s="22"/>
+    </row>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C41" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D40" s="24">
-        <f>+AVERAGE(D41:D42)</f>
-        <v>1.4999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="41" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C41" s="28" t="s">
+      <c r="D41" s="24">
+        <f>+AVERAGE(D42:D43)</f>
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C42" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="D41" s="25">
-        <v>0.03</v>
-      </c>
-    </row>
-    <row r="42" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C42" s="28" t="s">
+      <c r="D42" s="25">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C43" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="D42" s="25">
+      <c r="D43" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C43" s="7"/>
-    </row>
-    <row r="44" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C44" s="7"/>
     </row>
-    <row r="45" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C45" s="7"/>
     </row>
-    <row r="46" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C46" s="7"/>
     </row>
-    <row r="47" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B47" s="63" t="s">
+        <v>590</v>
+      </c>
       <c r="C47" s="7"/>
     </row>
-    <row r="48" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C48" s="7"/>
-    </row>
-    <row r="49" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C49" s="7"/>
-    </row>
-    <row r="50" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C50" s="7"/>
-    </row>
-    <row r="51" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C51" s="7"/>
-    </row>
-    <row r="52" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C52" s="7"/>
-    </row>
-    <row r="53" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C53" s="7"/>
-    </row>
-    <row r="54" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C54" s="7"/>
-    </row>
-    <row r="55" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C55" s="7"/>
-    </row>
-    <row r="56" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C56" s="7"/>
-    </row>
-    <row r="57" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C57" s="7"/>
+    <row r="48" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B48" s="64" t="s">
+        <v>593</v>
+      </c>
+      <c r="C48" s="7" t="s">
+        <v>586</v>
+      </c>
+      <c r="D48" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B49" s="62"/>
+      <c r="C49" s="7" t="s">
+        <v>587</v>
+      </c>
+      <c r="D49" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C50" s="7" t="s">
+        <v>588</v>
+      </c>
+      <c r="D50" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C51" s="7" t="s">
+        <v>589</v>
+      </c>
+      <c r="D51" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C52" s="7" t="s">
+        <v>592</v>
+      </c>
+      <c r="D52" s="22">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="53" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C53" s="7" t="s">
+        <v>591</v>
+      </c>
+      <c r="D53" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C54"/>
+      <c r="D54"/>
+    </row>
+    <row r="55" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C55"/>
+      <c r="D55"/>
+    </row>
+    <row r="56" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C56"/>
+      <c r="D56"/>
+    </row>
+    <row r="57" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C57"/>
+      <c r="D57"/>
+    </row>
+    <row r="58" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C58"/>
+      <c r="D58"/>
+    </row>
+    <row r="59" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C59"/>
+      <c r="D59"/>
+    </row>
+    <row r="60" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C60"/>
+      <c r="D60"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -3589,19 +3700,7 @@
     <mergeCell ref="B19:C19"/>
     <mergeCell ref="B29:C29"/>
   </mergeCells>
-  <conditionalFormatting sqref="D3">
-    <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="0.5"/>
-        <cfvo type="num" val="1"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D5:D42">
+  <conditionalFormatting sqref="D48:D53 D3 D5:D43">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -3623,7 +3722,7 @@
   <dimension ref="B2:D45"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3648,7 +3747,7 @@
       </c>
       <c r="D3" s="22">
         <f>+AVERAGE(D5,D6,D9,D10,D16,D17,D20,D21,D24,D25,D26,D27,D30,D34,D38)</f>
-        <v>0.22999999999999998</v>
+        <v>0.24333333333333332</v>
       </c>
     </row>
     <row r="4" spans="2:4" s="11" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -3657,18 +3756,18 @@
       <c r="D4" s="21"/>
     </row>
     <row r="5" spans="2:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="62" t="s">
+      <c r="B5" s="61" t="s">
         <v>32</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>33</v>
       </c>
       <c r="D5" s="22">
-        <v>0.9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B6" s="62"/>
+      <c r="B6" s="61"/>
       <c r="C6" s="7" t="s">
         <v>585</v>
       </c>
@@ -3686,7 +3785,7 @@
       <c r="D8" s="22"/>
     </row>
     <row r="9" spans="2:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="61" t="s">
+      <c r="B9" s="60" t="s">
         <v>34</v>
       </c>
       <c r="C9" s="7" t="s">
@@ -3697,7 +3796,7 @@
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B10" s="61"/>
+      <c r="B10" s="60"/>
       <c r="C10" s="7" t="s">
         <v>36</v>
       </c>
@@ -3842,8 +3941,8 @@
         <v>47</v>
       </c>
       <c r="D30" s="22">
-        <f>+AVERAGE(D31:D33)</f>
-        <v>4.9999999999999996E-2</v>
+        <f>+AVERAGE(D31)</f>
+        <v>0.15</v>
       </c>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.3">
@@ -3875,7 +3974,7 @@
         <v>51</v>
       </c>
       <c r="D34" s="22">
-        <f>+AVERAGE(D35:D37)</f>
+        <f>+AVERAGE(D35)</f>
         <v>0</v>
       </c>
     </row>
@@ -3966,9 +4065,6 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <ignoredErrors>
-    <ignoredError sqref="D34" formulaRange="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
 
@@ -3976,7 +4072,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42E9B1B1-FF6A-4270-B100-DB5C0019BAE1}">
   <dimension ref="D2:H83"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A55" workbookViewId="0">
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Learning control advance: updated / OOP directory created and the OOP study started
</commit_message>
<xml_diff>
--- a/Learning Advance Control.xlsx
+++ b/Learning Advance Control.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USUARIO\GR\Software Development\Learning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28EBC7C9-381A-4881-A0AE-14EAA5CEDA6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FC5A5AD-E8C4-40E3-8CA0-13B53D73DA69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C28AFF7E-06EE-4EAA-BF3B-F70E2F389C99}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{C28AFF7E-06EE-4EAA-BF3B-F70E2F389C99}"/>
   </bookViews>
   <sheets>
     <sheet name="Language" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="748" uniqueCount="594">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="747" uniqueCount="593">
   <si>
     <t>Basic Syntax</t>
   </si>
@@ -2338,9 +2338,6 @@
   </si>
   <si>
     <t>Context Managers</t>
-  </si>
-  <si>
-    <t>HackerRank DataStructures Exercices</t>
   </si>
   <si>
     <t>-</t>
@@ -2612,7 +2609,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2657,12 +2654,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF7030A0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -2681,7 +2672,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
@@ -2834,21 +2825,8 @@
     <xf numFmtId="0" fontId="25" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
@@ -2859,8 +2837,20 @@
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3251,17 +3241,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E55BE2DC-6D03-4737-9A16-12A22A3E1488}">
-  <dimension ref="B2:H60"/>
+  <dimension ref="B2:H59"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" outlineLevelRow="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.109375" customWidth="1"/>
     <col min="2" max="2" width="29.21875" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.77734375" style="6" customWidth="1"/>
+    <col min="3" max="3" width="24.33203125" style="6" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.5546875" style="5" customWidth="1"/>
     <col min="5" max="5" width="1.77734375" customWidth="1"/>
   </cols>
@@ -3279,8 +3269,8 @@
         <v>57</v>
       </c>
       <c r="D3" s="22">
-        <f>+AVERAGE(D5,D6,D14,D16,D17,D15,D21,D22,D23,D24,D26,D27,D31,D36,D37,D38,D39)</f>
-        <v>0.63529411764705879</v>
+        <f>+AVERAGE(D5,D6,D14,D16,D17,D15,D21,D22,D23,D24,D26,D27,D30,D35,D36,D37,D38)</f>
+        <v>0.73823529411764699</v>
       </c>
     </row>
     <row r="4" spans="2:8" s="11" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -3308,7 +3298,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:8" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="C7" s="13" t="s">
         <v>2</v>
       </c>
@@ -3316,7 +3306,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:8" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="C8" s="13" t="s">
         <v>3</v>
       </c>
@@ -3325,7 +3315,7 @@
       </c>
       <c r="H8" s="26"/>
     </row>
-    <row r="9" spans="2:8" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="C9" s="13" t="s">
         <v>4</v>
       </c>
@@ -3333,7 +3323,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:8" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="C10" s="13" t="s">
         <v>5</v>
       </c>
@@ -3341,7 +3331,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:8" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="C11" s="13" t="s">
         <v>6</v>
       </c>
@@ -3349,7 +3339,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:8" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="C12" s="13" t="s">
         <v>11</v>
       </c>
@@ -3357,7 +3347,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:8" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="C13" s="13" t="s">
         <v>7</v>
       </c>
@@ -3366,7 +3356,7 @@
       </c>
       <c r="F13" s="26"/>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:8" collapsed="1" x14ac:dyDescent="0.3">
       <c r="C14" s="7" t="s">
         <v>8</v>
       </c>
@@ -3403,10 +3393,10 @@
       <c r="D18" s="23"/>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B19" s="65" t="s">
+      <c r="B19" s="61" t="s">
         <v>574</v>
       </c>
-      <c r="C19" s="65"/>
+      <c r="C19" s="61"/>
       <c r="D19" s="22">
         <v>1</v>
       </c>
@@ -3417,7 +3407,7 @@
       <c r="D20" s="23"/>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B21" s="59" t="s">
+      <c r="B21" s="60" t="s">
         <v>21</v>
       </c>
       <c r="C21" s="7" t="s">
@@ -3428,7 +3418,7 @@
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B22" s="59"/>
+      <c r="B22" s="60"/>
       <c r="C22" s="7" t="s">
         <v>15</v>
       </c>
@@ -3453,28 +3443,27 @@
       </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C25" s="7" t="s">
-        <v>584</v>
+      <c r="C25" s="64" t="s">
+        <v>583</v>
       </c>
       <c r="D25" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C26" s="57" t="s">
+      <c r="C26" s="64" t="s">
         <v>18</v>
       </c>
       <c r="D26" s="22">
-        <v>0.1</v>
-      </c>
-      <c r="E26" s="56"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C27" s="57" t="s">
+      <c r="C27" s="64" t="s">
         <v>19</v>
       </c>
       <c r="D27" s="22">
-        <v>0.15</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.3">
@@ -3482,73 +3471,72 @@
       <c r="D28" s="23"/>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B29" s="65" t="s">
-        <v>582</v>
-      </c>
-      <c r="C29" s="65"/>
-      <c r="D29" s="22">
-        <v>0</v>
-      </c>
+      <c r="C29" s="7"/>
+      <c r="D29" s="23"/>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C30" s="7"/>
-      <c r="D30" s="23"/>
-    </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B31" s="9" t="s">
+      <c r="B30" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C31" s="7" t="s">
+      <c r="C30" s="7" t="s">
         <v>25</v>
       </c>
+      <c r="D30" s="22">
+        <f>+AVERAGE(D31:D34)</f>
+        <v>0.15000000000000002</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="C31" s="13" t="s">
+        <v>22</v>
+      </c>
       <c r="D31" s="22">
-        <f>+AVERAGE(D32:D35)</f>
-        <v>0.15000000000000002</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="32" spans="2:6" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="C32" s="13" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D32" s="22">
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="33" spans="2:4" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="C33" s="13" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D33" s="22">
-        <v>0.15</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="34" spans="2:4" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="C34" s="13" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D34" s="22">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="35" spans="2:4" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="C35" s="13" t="s">
-        <v>27</v>
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C35" s="7" t="s">
+        <v>26</v>
       </c>
       <c r="D35" s="22">
-        <v>0.05</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C36" s="7" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D36" s="22">
-        <v>0</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C37" s="7" t="s">
-        <v>28</v>
+        <v>580</v>
       </c>
       <c r="D37" s="22">
         <v>0.2</v>
@@ -3556,48 +3544,43 @@
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C38" s="7" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="D38" s="22">
-        <v>0.2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C39" s="7" t="s">
-        <v>581</v>
-      </c>
-      <c r="D39" s="22">
-        <v>0</v>
-      </c>
+      <c r="C39" s="7"/>
+      <c r="D39" s="22"/>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C40" s="7"/>
-      <c r="D40" s="22"/>
+      <c r="C40" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D40" s="24">
+        <f>+AVERAGE(D41:D42)</f>
+        <v>0.05</v>
+      </c>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C41" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D41" s="24">
-        <f>+AVERAGE(D42:D43)</f>
-        <v>0.05</v>
+      <c r="C41" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="D41" s="25">
+        <v>0.1</v>
       </c>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C42" s="28" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D42" s="25">
-        <v>0.1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C43" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="D43" s="25">
-        <v>0</v>
-      </c>
+      <c r="C43" s="7"/>
     </row>
     <row r="44" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C44" s="7"/>
@@ -3606,18 +3589,24 @@
       <c r="C45" s="7"/>
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B46" s="58" t="s">
+        <v>589</v>
+      </c>
       <c r="C46" s="7"/>
     </row>
     <row r="47" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B47" s="63" t="s">
-        <v>590</v>
-      </c>
-      <c r="C47" s="7"/>
+      <c r="B47" s="59" t="s">
+        <v>592</v>
+      </c>
+      <c r="C47" s="7" t="s">
+        <v>585</v>
+      </c>
+      <c r="D47" s="22">
+        <v>0</v>
+      </c>
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B48" s="64" t="s">
-        <v>593</v>
-      </c>
+      <c r="B48" s="57"/>
       <c r="C48" s="7" t="s">
         <v>586</v>
       </c>
@@ -3625,8 +3614,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B49" s="62"/>
+    <row r="49" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C49" s="7" t="s">
         <v>587</v>
       </c>
@@ -3634,7 +3622,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C50" s="7" t="s">
         <v>588</v>
       </c>
@@ -3642,65 +3630,56 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C51" s="7" t="s">
-        <v>589</v>
+        <v>591</v>
       </c>
       <c r="D51" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C52" s="7" t="s">
+        <v>590</v>
+      </c>
+      <c r="D52" s="22">
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C52" s="7" t="s">
-        <v>592</v>
-      </c>
-      <c r="D52" s="22">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C53" s="7" t="s">
-        <v>591</v>
-      </c>
-      <c r="D53" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C53"/>
+      <c r="D53"/>
+    </row>
+    <row r="54" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C54"/>
       <c r="D54"/>
     </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C55"/>
       <c r="D55"/>
     </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C56"/>
       <c r="D56"/>
     </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C57"/>
       <c r="D57"/>
     </row>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C58"/>
       <c r="D58"/>
     </row>
-    <row r="59" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C59"/>
       <c r="D59"/>
     </row>
-    <row r="60" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C60"/>
-      <c r="D60"/>
-    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="2">
     <mergeCell ref="B21:B22"/>
     <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B29:C29"/>
   </mergeCells>
-  <conditionalFormatting sqref="D48:D53 D3 D5:D43">
+  <conditionalFormatting sqref="D47:D52 D3 D5:D42">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -3756,7 +3735,7 @@
       <c r="D4" s="21"/>
     </row>
     <row r="5" spans="2:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="61" t="s">
+      <c r="B5" s="63" t="s">
         <v>32</v>
       </c>
       <c r="C5" s="7" t="s">
@@ -3767,9 +3746,9 @@
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B6" s="61"/>
+      <c r="B6" s="63"/>
       <c r="C6" s="7" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="D6" s="22">
         <v>0.1</v>
@@ -3785,7 +3764,7 @@
       <c r="D8" s="22"/>
     </row>
     <row r="9" spans="2:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="60" t="s">
+      <c r="B9" s="62" t="s">
         <v>34</v>
       </c>
       <c r="C9" s="7" t="s">
@@ -3796,7 +3775,7 @@
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B10" s="60"/>
+      <c r="B10" s="62"/>
       <c r="C10" s="7" t="s">
         <v>36</v>
       </c>
@@ -3817,16 +3796,16 @@
       <c r="C12" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="D12" s="58" t="s">
-        <v>583</v>
+      <c r="D12" s="56" t="s">
+        <v>582</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C13" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="D13" s="58" t="s">
-        <v>583</v>
+      <c r="D13" s="56" t="s">
+        <v>582</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
LAC Updated / Two Turing coding test reviewed
</commit_message>
<xml_diff>
--- a/Learning Advance Control.xlsx
+++ b/Learning Advance Control.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USUARIO\GR\Software Development\Learning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{165A4E9E-E413-458D-A34F-322594AE0F28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D92983B9-E695-462F-AB40-38626C22236B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{C28AFF7E-06EE-4EAA-BF3B-F70E2F389C99}"/>
+    <workbookView xWindow="0" yWindow="24" windowWidth="23016" windowHeight="12336" xr2:uid="{C28AFF7E-06EE-4EAA-BF3B-F70E2F389C99}"/>
   </bookViews>
   <sheets>
     <sheet name="Language" sheetId="1" r:id="rId1"/>
@@ -3225,7 +3225,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E55BE2DC-6D03-4737-9A16-12A22A3E1488}">
   <dimension ref="B2:H54"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -4003,7 +4003,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42E9B1B1-FF6A-4270-B100-DB5C0019BAE1}">
   <dimension ref="D2:H83"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A55" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A55" workbookViewId="0">
       <selection activeCell="F78" sqref="F78"/>
     </sheetView>
   </sheetViews>

</xml_diff>